<commit_message>
stats comparisons of ranunculus rhomboides
</commit_message>
<xml_diff>
--- a/ranun.rhomb_StatsComparison.xlsx
+++ b/ranun.rhomb_StatsComparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moin2\OneDrive\Documents\Bareground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AFE44D-3717-4E95-AD10-83F0406C4A7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFF55F0-F2BD-4EFA-92E9-4218278E2C16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5124" yWindow="1404" windowWidth="17280" windowHeight="8964" xr2:uid="{4FAABD45-D5C4-4811-9EBE-C38E444A2CC8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4FAABD45-D5C4-4811-9EBE-C38E444A2CC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
   <si>
     <t>Statistic</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>No SPDX</t>
+  </si>
+  <si>
+    <t>No AGDU</t>
   </si>
 </sst>
 </file>
@@ -573,21 +576,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E444ED6-417E-4F99-839F-D31873BCE2D3}">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.109375" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="18.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -601,24 +605,27 @@
         <v>55</v>
       </c>
       <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -631,11 +638,14 @@
       <c r="D3">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3">
+        <v>2.8069999999999999</v>
+      </c>
+      <c r="F3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -648,8 +658,11 @@
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -662,11 +675,14 @@
       <c r="D5">
         <v>0.94199999999999995</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5">
+        <v>9.4E-2</v>
+      </c>
+      <c r="F5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -680,16 +696,19 @@
       <c r="D6">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6">
+        <v>2.8069999999999999</v>
+      </c>
+      <c r="F6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -702,8 +721,11 @@
       <c r="D8">
         <v>34.655999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>25.817</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -716,8 +738,11 @@
       <c r="D9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -730,16 +755,19 @@
       <c r="D10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -752,11 +780,14 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="F12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -769,16 +800,19 @@
       <c r="D13">
         <v>1.208</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="F13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -791,14 +825,17 @@
       <c r="D15">
         <v>755.73</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15">
+        <v>605.15200000000004</v>
+      </c>
+      <c r="F15" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -811,11 +848,14 @@
       <c r="D16">
         <v>773.505</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16">
+        <v>622.92700000000002</v>
+      </c>
+      <c r="F16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -828,16 +868,19 @@
       <c r="D17">
         <v>733.05700000000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>582.47900000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -850,8 +893,11 @@
       <c r="D19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -864,21 +910,24 @@
       <c r="D20">
         <v>0.94399999999999995</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20">
+        <v>0.106</v>
+      </c>
+      <c r="F20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -888,8 +937,11 @@
       <c r="D24">
         <v>0.74</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>0.44500000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -899,8 +951,11 @@
       <c r="D25">
         <v>2.68</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>0.80400000000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -910,13 +965,16 @@
       <c r="D26">
         <v>7.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>0.42199999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -927,7 +985,7 @@
         <v>0.77800000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -938,7 +996,7 @@
         <v>3.492</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -949,41 +1007,50 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>22</v>
       </c>
       <c r="B32">
         <v>0.309</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32">
+        <v>1.101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>23</v>
       </c>
       <c r="B33">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <v>1.4330000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>10</v>
       </c>
       <c r="B34">
         <v>0.81799999999999995</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <v>0.152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -994,7 +1061,7 @@
         <v>0.17799999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -1005,7 +1072,7 @@
         <v>1.397</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -1016,12 +1083,12 @@
         <v>0.16200000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -1031,8 +1098,11 @@
       <c r="C40">
         <v>0.47099999999999997</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <v>0.56599999999999995</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>23</v>
       </c>
@@ -1042,8 +1112,11 @@
       <c r="C41">
         <v>2.86</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E41">
+        <v>3.3620000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -1053,13 +1126,16 @@
       <c r="C42">
         <v>4.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E42">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -1069,8 +1145,11 @@
       <c r="D44">
         <v>-0.20100000000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E44">
+        <v>0.36899999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -1080,8 +1159,11 @@
       <c r="D45">
         <v>-0.76800000000000002</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E45">
+        <v>1.5509999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -1091,13 +1173,16 @@
       <c r="D46">
         <v>0.442</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E46">
+        <v>0.121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>22</v>
       </c>
@@ -1107,8 +1192,11 @@
       <c r="C48">
         <v>0.29499999999999998</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E48">
+        <v>0.40699999999999997</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>23</v>
       </c>
@@ -1118,8 +1206,11 @@
       <c r="C49">
         <v>0.84</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E49">
+        <v>0.75900000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -1129,13 +1220,16 @@
       <c r="C50">
         <v>0.40100000000000002</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E50">
+        <v>0.44800000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>22</v>
       </c>
@@ -1149,7 +1243,7 @@
         <v>1.042</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>23</v>
       </c>
@@ -1163,7 +1257,7 @@
         <v>3.052</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -1177,12 +1271,12 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>40</v>
       </c>
@@ -1192,8 +1286,11 @@
       <c r="D56">
         <v>0.501</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E56">
+        <v>0.40300000000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>41</v>
       </c>
@@ -1203,8 +1300,11 @@
       <c r="C57">
         <v>0.53600000000000003</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E57">
+        <v>0.47099999999999997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>42</v>
       </c>
@@ -1217,13 +1317,16 @@
       <c r="D58">
         <v>0.65300000000000002</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E58">
+        <v>0.438</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>44</v>
       </c>
@@ -1233,8 +1336,11 @@
       <c r="D60">
         <v>0.85099999999999998</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E60">
+        <v>1.1639999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>10</v>
       </c>
@@ -1244,8 +1350,11 @@
       <c r="D61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>45</v>
       </c>
@@ -1255,8 +1364,11 @@
       <c r="C62">
         <v>1.139</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E62">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -1266,8 +1378,11 @@
       <c r="C63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>46</v>
       </c>
@@ -1278,7 +1393,7 @@
         <v>0.84399999999999997</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>10</v>
       </c>
@@ -1289,7 +1404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>47</v>
       </c>
@@ -1300,7 +1415,7 @@
         <v>1.0529999999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>10</v>
       </c>
@@ -1311,26 +1426,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>48</v>
       </c>
       <c r="B68">
         <v>0.89100000000000001</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E68">
+        <v>1.4059999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>10</v>
       </c>
       <c r="B69">
         <v>6.3E-2</v>
       </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" location="tldr-summary-of-global-fit-statistics" display="https://psu-psychology.github.io/psy-597-SEM/08_fit/sem_fit_modification.html - tldr-summary-of-global-fit-statistics" xr:uid="{9014F191-A100-4A45-B79B-BAE5BE5036B2}"/>
-    <hyperlink ref="F15" r:id="rId2" xr:uid="{2025C587-7378-498F-BA29-B39DE6ACC7AA}"/>
+    <hyperlink ref="G2" r:id="rId1" location="tldr-summary-of-global-fit-statistics" display="https://psu-psychology.github.io/psy-597-SEM/08_fit/sem_fit_modification.html - tldr-summary-of-global-fit-statistics" xr:uid="{9014F191-A100-4A45-B79B-BAE5BE5036B2}"/>
+    <hyperlink ref="G15" r:id="rId2" xr:uid="{2025C587-7378-498F-BA29-B39DE6ACC7AA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>